<commit_message>
/ ‘RPG-Table Top/Pathfinder/Drew-MarchWest/Brewing Potions.xlsx’
</commit_message>
<xml_diff>
--- a/RPG-Table Top/Pathfinder/Drew-MarchWest/Brewing Potions.xlsx
+++ b/RPG-Table Top/Pathfinder/Drew-MarchWest/Brewing Potions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phoenix\Documents\Table Top Games\PCGen6.08.00RC8\6.08.00RC8\characters\Shillvei Fadvess\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tat36\SparkleShare\sparkle\RPG-Table Top\Pathfinder\Drew-MarchWest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11400" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11400"/>
   </bookViews>
   <sheets>
     <sheet name="Potions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="292">
   <si>
     <t>Potion Spell Name</t>
   </si>
@@ -893,6 +893,15 @@
   </si>
   <si>
     <t>Make a Spellcraft or Craft (alchemy) check against a DC of 5 + Caster Level</t>
+  </si>
+  <si>
+    <t>2 AC</t>
+  </si>
+  <si>
+    <t>3 AC</t>
+  </si>
+  <si>
+    <t>4 AC</t>
   </si>
 </sst>
 </file>
@@ -1304,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,26 +1590,26 @@
         <v>20</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" ref="F7:F52" si="1">(B7*C7*50)</f>
+        <f t="shared" ref="F7:F60" si="1">(B7*C7*50)</f>
         <v>50</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" ref="G7:G52" si="2">F7-(F7*0.05)</f>
+        <f t="shared" ref="G7:G60" si="2">F7-(F7*0.05)</f>
         <v>47.5</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" ref="H7:H52" si="3">G7/2</f>
+        <f t="shared" ref="H7:H60" si="3">G7/2</f>
         <v>23.75</v>
       </c>
       <c r="I7" s="4">
         <v>2</v>
       </c>
       <c r="J7" s="3">
-        <f t="shared" ref="J7:J52" si="4">I7/2</f>
+        <f t="shared" ref="J7:J60" si="4">I7/2</f>
         <v>1</v>
       </c>
       <c r="K7" s="4">
-        <f t="shared" ref="K7:K52" si="5">5+C7</f>
+        <f t="shared" ref="K7:K60" si="5">5+C7</f>
         <v>6</v>
       </c>
     </row>
@@ -1973,7 +1982,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
@@ -2014,7 +2023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -2055,7 +2064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
@@ -2096,7 +2105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -2137,7 +2146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -2178,7 +2187,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>3</v>
       </c>
@@ -2219,7 +2228,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -2260,7 +2269,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>3</v>
       </c>
@@ -2301,7 +2310,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>4</v>
       </c>
@@ -2341,8 +2350,11 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>4</v>
       </c>
@@ -2382,8 +2394,11 @@
         <f t="shared" ref="K26" si="19">5+C26</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>4</v>
       </c>
@@ -2423,8 +2438,11 @@
         <f t="shared" ref="K27:K29" si="21">5+C27</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>4</v>
       </c>
@@ -2464,8 +2482,11 @@
         <f t="shared" si="21"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>4</v>
       </c>
@@ -2505,8 +2526,11 @@
         <f t="shared" si="21"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>4</v>
       </c>
@@ -2546,8 +2570,11 @@
         <f t="shared" ref="K30:K32" si="23">5+C30</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>4</v>
       </c>
@@ -2587,8 +2614,11 @@
         <f t="shared" si="23"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>4</v>
       </c>
@@ -2628,6 +2658,9 @@
         <f t="shared" si="23"/>
         <v>14</v>
       </c>
+      <c r="L32" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -2968,7 +3001,7 @@
         <v>2</v>
       </c>
       <c r="D41" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>22</v>
@@ -3273,85 +3306,84 @@
         <v>4</v>
       </c>
       <c r="K48" s="4">
-        <f t="shared" ref="K48" si="31">5+C48</f>
+        <f t="shared" ref="K48:K49" si="31">5+C48</f>
         <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="5"/>
+      <c r="A49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="4">
+        <v>2</v>
+      </c>
+      <c r="C49" s="4">
+        <v>10</v>
+      </c>
+      <c r="D49" s="4">
+        <v>10</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F49" s="4">
+        <f>(B49*C49*50)</f>
+        <v>1000</v>
+      </c>
+      <c r="G49" s="4">
+        <f t="shared" si="2"/>
+        <v>950</v>
+      </c>
+      <c r="H49" s="3">
+        <f t="shared" si="3"/>
+        <v>475</v>
+      </c>
+      <c r="I49" s="4">
+        <v>8</v>
+      </c>
+      <c r="J49" s="3">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="K49" s="4">
+        <f t="shared" si="31"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="5"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B51" s="4">
         <v>3</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C51" s="4">
         <v>3</v>
       </c>
-      <c r="D50" s="4">
-        <v>5</v>
-      </c>
-      <c r="E50" s="4" t="s">
+      <c r="D51" s="4">
+        <v>3</v>
+      </c>
+      <c r="E51" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F50" s="4">
+      <c r="F51" s="4">
         <f t="shared" si="1"/>
         <v>450</v>
       </c>
-      <c r="G50" s="4">
-        <f t="shared" si="2"/>
-        <v>427.5</v>
-      </c>
-      <c r="H50" s="3">
-        <f t="shared" si="3"/>
-        <v>213.75</v>
-      </c>
-      <c r="I50" s="4">
-        <v>8</v>
-      </c>
-      <c r="J50" s="3">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="K50" s="4">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B51" s="2">
-        <v>3</v>
-      </c>
-      <c r="C51" s="2">
-        <v>3</v>
-      </c>
-      <c r="D51" s="2">
-        <f>1*C51</f>
-        <v>3</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51" s="2">
-        <f t="shared" si="1"/>
-        <v>450</v>
-      </c>
-      <c r="G51" s="2">
+      <c r="G51" s="4">
         <f t="shared" si="2"/>
         <v>427.5</v>
       </c>
@@ -3359,46 +3391,43 @@
         <f t="shared" si="3"/>
         <v>213.75</v>
       </c>
-      <c r="I51" s="2">
+      <c r="I51" s="4">
         <v>8</v>
       </c>
       <c r="J51" s="3">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="K51" s="2">
+      <c r="K51" s="4">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A52" s="4"/>
       <c r="B52" s="4">
         <v>3</v>
       </c>
       <c r="C52" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D52" s="4">
-        <f>10*C52</f>
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F52" s="4">
         <f t="shared" si="1"/>
-        <v>450</v>
+        <v>600</v>
       </c>
       <c r="G52" s="4">
         <f t="shared" si="2"/>
-        <v>427.5</v>
+        <v>570</v>
       </c>
       <c r="H52" s="3">
         <f t="shared" si="3"/>
-        <v>213.75</v>
+        <v>285</v>
       </c>
       <c r="I52" s="4">
         <v>8</v>
@@ -3408,6 +3437,316 @@
         <v>4</v>
       </c>
       <c r="K52" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4">
+        <v>3</v>
+      </c>
+      <c r="C53" s="4">
+        <v>5</v>
+      </c>
+      <c r="D53" s="4">
+        <v>5</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" s="4">
+        <f t="shared" si="1"/>
+        <v>750</v>
+      </c>
+      <c r="G53" s="4">
+        <f t="shared" si="2"/>
+        <v>712.5</v>
+      </c>
+      <c r="H53" s="3">
+        <f t="shared" si="3"/>
+        <v>356.25</v>
+      </c>
+      <c r="I53" s="4">
+        <v>8</v>
+      </c>
+      <c r="J53" s="3">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="K53" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4">
+        <v>3</v>
+      </c>
+      <c r="C54" s="4">
+        <v>6</v>
+      </c>
+      <c r="D54" s="4">
+        <v>6</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F54" s="4">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+      <c r="G54" s="4">
+        <f t="shared" si="2"/>
+        <v>855</v>
+      </c>
+      <c r="H54" s="3">
+        <f t="shared" si="3"/>
+        <v>427.5</v>
+      </c>
+      <c r="I54" s="4">
+        <v>8</v>
+      </c>
+      <c r="J54" s="3">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="K54" s="4">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4">
+        <v>3</v>
+      </c>
+      <c r="C55" s="4">
+        <v>7</v>
+      </c>
+      <c r="D55" s="4">
+        <v>7</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F55" s="4">
+        <f t="shared" si="1"/>
+        <v>1050</v>
+      </c>
+      <c r="G55" s="4">
+        <f t="shared" si="2"/>
+        <v>997.5</v>
+      </c>
+      <c r="H55" s="3">
+        <f t="shared" si="3"/>
+        <v>498.75</v>
+      </c>
+      <c r="I55" s="4">
+        <v>16</v>
+      </c>
+      <c r="J55" s="3">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="K55" s="4">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4">
+        <v>3</v>
+      </c>
+      <c r="C56" s="4">
+        <v>8</v>
+      </c>
+      <c r="D56" s="4">
+        <v>8</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" s="4">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="G56" s="4">
+        <f t="shared" si="2"/>
+        <v>1140</v>
+      </c>
+      <c r="H56" s="3">
+        <f t="shared" si="3"/>
+        <v>570</v>
+      </c>
+      <c r="I56" s="4">
+        <v>16</v>
+      </c>
+      <c r="J56" s="3">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="K56" s="4">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4">
+        <v>3</v>
+      </c>
+      <c r="C57" s="4">
+        <v>9</v>
+      </c>
+      <c r="D57" s="4">
+        <v>9</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F57" s="4">
+        <f t="shared" si="1"/>
+        <v>1350</v>
+      </c>
+      <c r="G57" s="4">
+        <f t="shared" si="2"/>
+        <v>1282.5</v>
+      </c>
+      <c r="H57" s="3">
+        <f t="shared" si="3"/>
+        <v>641.25</v>
+      </c>
+      <c r="I57" s="4">
+        <v>16</v>
+      </c>
+      <c r="J57" s="3">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="K57" s="4">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4">
+        <v>3</v>
+      </c>
+      <c r="C58" s="4">
+        <v>10</v>
+      </c>
+      <c r="D58" s="4">
+        <v>10</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F58" s="4">
+        <f t="shared" si="1"/>
+        <v>1500</v>
+      </c>
+      <c r="G58" s="4">
+        <f t="shared" si="2"/>
+        <v>1425</v>
+      </c>
+      <c r="H58" s="3">
+        <f t="shared" si="3"/>
+        <v>712.5</v>
+      </c>
+      <c r="I58" s="4">
+        <v>16</v>
+      </c>
+      <c r="J58" s="3">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="K58" s="4">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" s="2">
+        <v>3</v>
+      </c>
+      <c r="C59" s="2">
+        <v>3</v>
+      </c>
+      <c r="D59" s="2">
+        <f>1*C59</f>
+        <v>3</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F59" s="2">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="G59" s="2">
+        <f t="shared" si="2"/>
+        <v>427.5</v>
+      </c>
+      <c r="H59" s="3">
+        <f t="shared" si="3"/>
+        <v>213.75</v>
+      </c>
+      <c r="I59" s="2">
+        <v>8</v>
+      </c>
+      <c r="J59" s="3">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="K59" s="2">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" s="4">
+        <v>3</v>
+      </c>
+      <c r="C60" s="4">
+        <v>3</v>
+      </c>
+      <c r="D60" s="4">
+        <f>10*C60</f>
+        <v>30</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F60" s="4">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="G60" s="4">
+        <f t="shared" si="2"/>
+        <v>427.5</v>
+      </c>
+      <c r="H60" s="3">
+        <f t="shared" si="3"/>
+        <v>213.75</v>
+      </c>
+      <c r="I60" s="4">
+        <v>8</v>
+      </c>
+      <c r="J60" s="3">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="K60" s="4">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
@@ -6983,7 +7322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>